<commit_message>
Refactor: Implement services for admin functionality
</commit_message>
<xml_diff>
--- a/testImport.xlsx
+++ b/testImport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Дмитрий\Desktop\Интравижен\MyDrinkCatalog\DrinkCatalog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\MyDrinkCatalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F990B9B5-C6B5-459A-9C15-265C98C8DFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920A1B7C-231C-439E-90C9-245434AB70D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="7395" windowWidth="25095" windowHeight="15435" xr2:uid="{4DE63CC5-0C1F-434A-9344-64A977726D66}"/>
+    <workbookView xWindow="11025" yWindow="11610" windowWidth="25095" windowHeight="15435" xr2:uid="{4DE63CC5-0C1F-434A-9344-64A977726D66}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>ImageUrl</t>
   </si>
   <si>
-    <t>\Img\Drink\11756b73-11cf-4971-ac21-784a2fe88fb0.jpg</t>
+    <t>\Img\Drink\0154118d-a578-4d20-a6ef-963695d6dd7c.jpg</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>